<commit_message>
CSV to xlsx with gui
</commit_message>
<xml_diff>
--- a/文字コードテスト/UTF-8.xlsx
+++ b/文字コードテスト/UTF-8.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,48 +436,54 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>col1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>col2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>col3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>time</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>weight</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>radius</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
         <v>0.9</v>
@@ -485,10 +491,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" t="n">
         <v>0.9</v>
@@ -496,32 +502,32 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C6" t="n">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C7" t="n">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C8" t="n">
         <v>0.88</v>
@@ -529,10 +535,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C9" t="n">
         <v>0.88</v>
@@ -540,21 +546,21 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" t="n">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" t="n">
         <v>0.87</v>
@@ -562,12 +568,23 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="n">
         <v>66</v>
       </c>
       <c r="C12" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" t="n">
+        <v>66</v>
+      </c>
+      <c r="C13" t="n">
         <v>0.87</v>
       </c>
     </row>

</xml_diff>